<commit_message>
Litle progress in executing old tests
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/JavaTestFramework/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B181F51-F8AF-9D42-A658-08E9F3AAB91A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>Tag</t>
   </si>
@@ -287,19 +293,28 @@
   </si>
   <si>
     <t>MSc Management CRO PTD 201819 for student application</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRELOGINURL</t>
+  </si>
+  <si>
+    <t>https://staging.bppdigital.buildempire.app/account</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREURL</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINURL</t>
+  </si>
+  <si>
+    <t>https://admin.staging.bppdigital.buildempire.app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,13 +327,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,355 +341,56 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF007DD6"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -695,251 +411,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -949,17 +426,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -967,65 +444,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1283,27 +720,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="45.4296875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="11"/>
+    <col min="1" max="1" width="38.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1325,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -1336,7 +773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1380,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1391,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -1402,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -1413,7 +850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -1424,7 +861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
@@ -1446,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
@@ -1457,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
@@ -1468,7 +905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1479,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1490,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" s="7" customFormat="1" spans="1:3">
+    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" s="7" customFormat="1" spans="1:3">
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1512,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="1" spans="1:3">
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1523,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="1" spans="1:3">
+    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1534,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" s="7" customFormat="1" spans="1:3">
+    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
@@ -1545,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" s="7" customFormat="1" spans="1:3">
+    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
@@ -1556,7 +993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" s="7" customFormat="1" spans="1:3">
+    <row r="24" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
@@ -1567,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" s="7" customFormat="1" spans="1:3">
+    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1578,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
@@ -1589,7 +1026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>52</v>
       </c>
@@ -1602,34 +1039,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="samuelslade@bpp.com "/>
-    <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
-    <hyperlink ref="B24" r:id="rId1" display="neo4j"/>
-    <hyperlink ref="B26" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B26" r:id="rId4" tooltip="mailto:craigolivant@bpp.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1651,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1662,7 +1097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1673,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1685,29 +1120,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1718,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -1729,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
@@ -1740,7 +1173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>64</v>
       </c>
@@ -1751,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -1762,7 +1195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -1773,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
@@ -1784,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
@@ -1795,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -1806,7 +1239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -1817,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:3">
+    <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1828,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>80</v>
       </c>
@@ -1839,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -1850,7 +1283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -1861,42 +1294,73 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
-    <hyperlink ref="B3" r:id="rId1" display=" http://noahqa-bpp-13fd3e55188.cs17.force.com/rfi"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://bpp-test.apolloglobal.int/registration/login" tooltip="Follow link"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://bpp-test.apolloglobal.int/ncas"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://bpp-test.apolloglobal.int/ncas/login?service=https://bpp-fusion-test.apolloglobal.int/ncas/sso-login"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://bpp-fusion-test.apolloglobal.int/vle/login/index.php?authCAS=NOCAS"/>
-    <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
-    <hyperlink ref="B13" r:id="rId8" display="http://pf-services-qa-1697893966.eu-west-2.elb.amazonaws.com"/>
-    <hyperlink ref="B14" r:id="rId9" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="Follow link" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.4296875" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1918,7 +1382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
@@ -1930,7 +1394,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change structure and made some cleanup
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/JavaTestFramework/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A61882-4376-EA4F-A8E1-4F3A17DB2499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19900" windowHeight="12500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="Links" sheetId="2" r:id="rId3"/>
     <sheet name="Validdata" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
   <si>
     <t>Tag</t>
   </si>
@@ -320,19 +326,49 @@
   </si>
   <si>
     <t>MSc Management CRO PTD 201819 for student application</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINUSER</t>
+  </si>
+  <si>
+    <t>apprenticeships@bpptest.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>Test Password003!</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERINUSER</t>
+  </si>
+  <si>
+    <t>waltdisney@mailinator.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERPASSWORD</t>
+  </si>
+  <si>
+    <t>Testing WALT 2018</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINUSER</t>
+  </si>
+  <si>
+    <t>neilsteward@outlook.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>I am really really bored now!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,13 +381,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -359,14 +395,14 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -374,7 +410,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -382,348 +418,33 @@
       <sz val="11"/>
       <color rgb="FF007DD6"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -744,251 +465,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,17 +480,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1018,65 +500,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="20% — Акцент3" xfId="1" builtinId="38"/>
-    <cellStyle name="Денежный [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% — Акцент5" xfId="3" builtinId="47"/>
-    <cellStyle name="Хороший" xfId="4" builtinId="26"/>
-    <cellStyle name="Запятая [0]" xfId="5" builtinId="6"/>
-    <cellStyle name="Денежный" xfId="6" builtinId="4"/>
-    <cellStyle name="Запятая" xfId="7" builtinId="3"/>
-    <cellStyle name="40% — Акцент6" xfId="8" builtinId="51"/>
-    <cellStyle name="Процент" xfId="9" builtinId="5"/>
-    <cellStyle name="20% — Акцент2" xfId="10" builtinId="34"/>
-    <cellStyle name="Итого" xfId="11" builtinId="25"/>
-    <cellStyle name="Вывод" xfId="12" builtinId="21"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8"/>
-    <cellStyle name="Примечание" xfId="14" builtinId="10"/>
-    <cellStyle name="40% — Акцент4" xfId="15" builtinId="43"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9"/>
-    <cellStyle name="Предупреждающий текст" xfId="17" builtinId="11"/>
-    <cellStyle name="Заголовок" xfId="18" builtinId="15"/>
-    <cellStyle name="Пояснительный текст" xfId="19" builtinId="53"/>
-    <cellStyle name="Заголовок 1" xfId="20" builtinId="16"/>
-    <cellStyle name="Заголовок 2" xfId="21" builtinId="17"/>
-    <cellStyle name="Заголовок 3" xfId="22" builtinId="18"/>
-    <cellStyle name="Заголовок 4" xfId="23" builtinId="19"/>
-    <cellStyle name="Ввод" xfId="24" builtinId="20"/>
-    <cellStyle name="Проверить ячейку" xfId="25" builtinId="23"/>
-    <cellStyle name="Вычисление" xfId="26" builtinId="22"/>
-    <cellStyle name="Связанная ячейка" xfId="27" builtinId="24"/>
-    <cellStyle name="Плохой" xfId="28" builtinId="27"/>
-    <cellStyle name="Акцент5" xfId="29" builtinId="45"/>
-    <cellStyle name="Нейтральный" xfId="30" builtinId="28"/>
-    <cellStyle name="Акцент1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% — Акцент1" xfId="32" builtinId="30"/>
-    <cellStyle name="40% — Акцент1" xfId="33" builtinId="31"/>
-    <cellStyle name="20% — Акцент5" xfId="34" builtinId="46"/>
-    <cellStyle name="60% — Акцент1" xfId="35" builtinId="32"/>
-    <cellStyle name="Акцент2" xfId="36" builtinId="33"/>
-    <cellStyle name="40% — Акцент2" xfId="37" builtinId="35"/>
-    <cellStyle name="20% — Акцент6" xfId="38" builtinId="50"/>
-    <cellStyle name="60% — Акцент2" xfId="39" builtinId="36"/>
-    <cellStyle name="Акцент3" xfId="40" builtinId="37"/>
-    <cellStyle name="40% — Акцент3" xfId="41" builtinId="39"/>
-    <cellStyle name="60% — Акцент3" xfId="42" builtinId="40"/>
-    <cellStyle name="Акцент4" xfId="43" builtinId="41"/>
-    <cellStyle name="20% — Акцент4" xfId="44" builtinId="42"/>
-    <cellStyle name="60% — Акцент4" xfId="45" builtinId="44"/>
-    <cellStyle name="60% — Акцент5" xfId="46" builtinId="48"/>
-    <cellStyle name="Акцент6" xfId="47" builtinId="49"/>
-    <cellStyle name="60% — Акцент6" xfId="48" builtinId="52"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1334,27 +776,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C29"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1619047619048" style="13" customWidth="1"/>
-    <col min="2" max="2" width="45.5047619047619" style="13" customWidth="1"/>
-    <col min="3" max="3" width="44.1619047619048" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="8.66666666666667" style="13"/>
+    <col min="1" max="1" width="38.1640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -1376,7 +818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -1398,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -1409,7 +851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
@@ -1420,7 +862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -1431,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -1442,7 +884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
@@ -1453,7 +895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1464,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -1475,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
@@ -1486,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1530,7 +972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1541,7 +983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" s="7" customFormat="1" spans="1:3">
+    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1552,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" s="7" customFormat="1" spans="1:3">
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1563,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="1" spans="1:3">
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1574,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="1" spans="1:3">
+    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" s="7" customFormat="1" spans="1:3">
+    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
@@ -1596,7 +1038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" s="7" customFormat="1" spans="1:3">
+    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
@@ -1607,7 +1049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" s="7" customFormat="1" spans="1:3">
+    <row r="24" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
@@ -1618,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" s="7" customFormat="1" spans="1:3">
+    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1629,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
@@ -1640,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>52</v>
       </c>
@@ -1651,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>53</v>
       </c>
@@ -1662,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>55</v>
       </c>
@@ -1673,36 +1115,100 @@
         <v>5</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="samuelslade@bpp.com "/>
-    <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
-    <hyperlink ref="B24" r:id="rId1" display="neo4j"/>
-    <hyperlink ref="B26" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B26" r:id="rId4" tooltip="mailto:craigolivant@bpp.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1724,7 +1230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1735,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1746,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1758,29 +1264,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="26.1619047619048" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1791,7 +1295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
@@ -1802,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
@@ -1813,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -1824,7 +1328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -1835,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1846,7 +1350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
@@ -1857,7 +1361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
@@ -1868,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
@@ -1879,7 +1383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -1890,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:3">
+    <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>82</v>
       </c>
@@ -1901,7 +1405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>84</v>
       </c>
@@ -1912,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>86</v>
       </c>
@@ -1923,7 +1427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>88</v>
       </c>
@@ -1934,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1945,7 +1449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>92</v>
       </c>
@@ -1956,7 +1460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>93</v>
       </c>
@@ -1967,7 +1471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -1980,40 +1484,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
-    <hyperlink ref="B3" r:id="rId1" display=" http://noahqa-bpp-13fd3e55188.cs17.force.com/rfi"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://bpp-test.apolloglobal.int/registration/login" tooltip="Follow link"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://bpp-test.apolloglobal.int/ncas"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://bpp-test.apolloglobal.int/ncas/login?service=https://bpp-fusion-test.apolloglobal.int/ncas/sso-login"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://bpp-fusion-test.apolloglobal.int/vle/login/index.php?authCAS=NOCAS"/>
-    <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
-    <hyperlink ref="B13" r:id="rId8" display="http://pf-services-qa-1697893966.eu-west-2.elb.amazonaws.com"/>
-    <hyperlink ref="B14" r:id="rId9" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="Follow link" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="34.5047619047619" customWidth="1"/>
-    <col min="3" max="3" width="37.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>97</v>
       </c>
@@ -2035,7 +1537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
@@ -2047,7 +1549,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated StepDefinitions class; edited Locators; updated BasePage class.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/qa-automation-framework-poc/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079A4C6F-D46D-454A-BDAA-59B757C789AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19900" windowHeight="12500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="14460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -196,6 +190,42 @@
     <t>Password1!!!</t>
   </si>
   <si>
+    <t>BUILDEMPIREADMINUSER</t>
+  </si>
+  <si>
+    <t>apprenticeships@bpptest.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>Test Password003!</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERINUSER</t>
+  </si>
+  <si>
+    <t>waltdisney@mailinator.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIREMANAGERPASSWORD</t>
+  </si>
+  <si>
+    <t>Testing WALT 2018</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINUSER</t>
+  </si>
+  <si>
+    <t>neilsteward@outlook.com</t>
+  </si>
+  <si>
+    <t>BUILDEMPIRENEILADMINPASSWORD</t>
+  </si>
+  <si>
+    <t>I am really really bored now!!</t>
+  </si>
+  <si>
     <t>ENTER</t>
   </si>
   <si>
@@ -286,6 +316,9 @@
     <t>PRODUCTFACTORYURL</t>
   </si>
   <si>
+    <t>http://qa-products.bpp.com</t>
+  </si>
+  <si>
     <t>PRODUCTFACTORYDATABASEURL</t>
   </si>
   <si>
@@ -323,52 +356,19 @@
   </si>
   <si>
     <t>MSc Management CRO PTD 201819 for student application</t>
-  </si>
-  <si>
-    <t>BUILDEMPIREADMINUSER</t>
-  </si>
-  <si>
-    <t>apprenticeships@bpptest.com</t>
-  </si>
-  <si>
-    <t>BUILDEMPIREADMINPASSWORD</t>
-  </si>
-  <si>
-    <t>Test Password003!</t>
-  </si>
-  <si>
-    <t>BUILDEMPIREMANAGERINUSER</t>
-  </si>
-  <si>
-    <t>waltdisney@mailinator.com</t>
-  </si>
-  <si>
-    <t>BUILDEMPIREMANAGERPASSWORD</t>
-  </si>
-  <si>
-    <t>Testing WALT 2018</t>
-  </si>
-  <si>
-    <t>BUILDEMPIRENEILADMINUSER</t>
-  </si>
-  <si>
-    <t>neilsteward@outlook.com</t>
-  </si>
-  <si>
-    <t>BUILDEMPIRENEILADMINPASSWORD</t>
-  </si>
-  <si>
-    <t>I am really really bored now!!</t>
-  </si>
-  <si>
-    <t>http://qa-products.bpp.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,13 +381,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -395,14 +395,14 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -410,7 +410,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,33 +418,355 @@
       <sz val="11"/>
       <color rgb="FF007DD6"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -465,12 +787,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,45 +1041,94 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -776,27 +1386,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="13"/>
+    <col min="1" max="1" width="38.1619047619048" style="15" customWidth="1"/>
+    <col min="2" max="2" width="45.5047619047619" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44.1619047619048" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="8.66666666666667" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -807,161 +1417,161 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="C2" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="C3" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="C4" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="C5" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="C6" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="C8" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="C12" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="C13" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" s="7" customFormat="1" spans="1:3">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -972,7 +1582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" s="7" customFormat="1" spans="1:3">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -983,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" s="7" customFormat="1" spans="1:3">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -994,7 +1604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" s="7" customFormat="1" spans="1:3">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1005,7 +1615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" s="7" customFormat="1" spans="1:3">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1016,7 +1626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" s="7" customFormat="1" spans="1:3">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1027,18 +1637,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" s="7" customFormat="1" spans="1:3">
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" s="7" customFormat="1" spans="1:3">
       <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
@@ -1049,18 +1659,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" s="7" customFormat="1" spans="1:3">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" s="7" customFormat="1" spans="1:3">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1071,18 +1681,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="17" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="7" t="s">
         <v>52</v>
       </c>
@@ -1093,122 +1703,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="C28" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="16" t="s">
+      <c r="C29" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B26" r:id="rId4" tooltip="mailto:craigolivant@bpp.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B22" r:id="rId1" display="samuelslade@bpp.com "/>
+    <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
+    <hyperlink ref="B24" r:id="rId1" display="neo4j"/>
+    <hyperlink ref="B26" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,72 +1831,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>57</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="26.1619047619048" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1295,226 +1909,228 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" s="4" customFormat="1" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>89</v>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>94</v>
+        <v>103</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" tooltip="Follow link" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B14" r:id="rId9" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
+    <hyperlink ref="B3" r:id="rId1" display=" http://noahqa-bpp-13fd3e55188.cs17.force.com/rfi"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://bpp-test.apolloglobal.int/registration/login" tooltip="Follow link"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://bpp-test.apolloglobal.int/ncas"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://bpp-test.apolloglobal.int/ncas/login?service=https://bpp-fusion-test.apolloglobal.int/ncas/sso-login"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage"/>
+    <hyperlink ref="B8" r:id="rId6" display="http://bpp-fusion-test.apolloglobal.int/vle/login/index.php?authCAS=NOCAS"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
+    <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="34.5047619047619" customWidth="1"/>
+    <col min="3" max="3" width="37.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,29 +2141,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SpecialLocators.json: Added locator 'Product Factory Locked Applies To drop-down item'; Added locator 'Product Factory Financial Dimension list in Locations'; Added locator 'Product Factory Check Link Levels button'; Locators.json: Added locator 'Product Factory Choose Dimension Popup Item Type'; Added locator 'Product Factory Body of Webpage'; Common_MetaData.xlsx: Added 'Escape' Keyboard Shortcut; Added 'End' Keyboard Shortcut; FD_PageAndList_BPP-2487.feature: Added comments with Test Case names for each scenario; FD_PageAndList_BPP-2488.feature: Added comments with Test Case names for each scenario; FD_PageAndList_BPP-2489.feature: Added comments with Test Case names for each scenario; Created 'FD_EditValidation_BPP-3328.feature' file and created 2 from 3 scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14460" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="14310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
   <si>
     <t>Tag</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>BACK_SPACE</t>
+  </si>
+  <si>
+    <t>ESCAPE</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
   <si>
     <t>SALESFORCEURL</t>
@@ -363,12 +369,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,30 +435,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,47 +458,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,29 +520,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -559,7 +529,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -581,187 +580,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,24 +787,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -821,17 +802,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -862,6 +837,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -877,18 +870,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -906,132 +905,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1052,25 +1051,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1395,15 +1385,15 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1619047619048" style="15" customWidth="1"/>
-    <col min="2" max="2" width="45.5047619047619" style="15" customWidth="1"/>
-    <col min="3" max="3" width="44.1619047619048" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.66666666666667" style="15"/>
+    <col min="1" max="1" width="38.1619047619048" style="10" customWidth="1"/>
+    <col min="2" max="2" width="45.5047619047619" style="10" customWidth="1"/>
+    <col min="3" max="3" width="44.1619047619048" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="8.66666666666667" style="10"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1418,142 +1408,142 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1561,10 +1551,10 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1641,7 +1631,7 @@
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1663,7 +1653,7 @@
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1685,7 +1675,7 @@
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1704,90 +1694,90 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1807,13 +1797,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="16.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
@@ -1835,7 +1825,7 @@
       <c r="A2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1872,6 +1862,28 @@
         <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1887,7 +1899,7 @@
   <sheetPr/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1911,10 +1923,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1922,10 +1934,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1933,10 +1945,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1944,10 +1956,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1955,10 +1967,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1966,10 +1978,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1977,10 +1989,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1988,10 +2000,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1999,10 +2011,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2010,10 +2022,10 @@
     </row>
     <row r="11" s="4" customFormat="1" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -2021,10 +2033,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -2032,10 +2044,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -2043,56 +2055,56 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="10" t="s">
-        <v>102</v>
+      <c r="A15" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
-        <v>107</v>
+      <c r="A18" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2143,10 +2155,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2154,10 +2166,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
created test for CSA Workflow Alerts. updated TestParametersController to update EC in xpath
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14310" activeTab="1"/>
+    <workbookView windowWidth="28245" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
   <si>
     <t>Tag</t>
   </si>
@@ -52,18 +52,6 @@
     <t>BPPADMINPASSWORD</t>
   </si>
   <si>
-    <t>SELFREGUSER</t>
-  </si>
-  <si>
-    <t>tchin@apollo.edu</t>
-  </si>
-  <si>
-    <t>SELFREGPASSWORD</t>
-  </si>
-  <si>
-    <t>Apollo01!</t>
-  </si>
-  <si>
     <t>BPPPORTALUSER</t>
   </si>
   <si>
@@ -100,18 +88,6 @@
     <t>Welcome1!</t>
   </si>
   <si>
-    <t>OPENBRAVOUSER</t>
-  </si>
-  <si>
-    <t>BP5041772</t>
-  </si>
-  <si>
-    <t>OPENBRAVOPASSWORD</t>
-  </si>
-  <si>
-    <t>Ch102116</t>
-  </si>
-  <si>
     <t>BPPBANNERUSER</t>
   </si>
   <si>
@@ -224,6 +200,18 @@
   </si>
   <si>
     <t>I am really really bored now!!</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCSAUSER</t>
+  </si>
+  <si>
+    <t>nadineanja@yahoo.com</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCSAPASSWORD</t>
+  </si>
+  <si>
+    <t>Wake Up 19!</t>
   </si>
   <si>
     <t>ENTER</t>
@@ -369,12 +357,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,7 +417,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -443,31 +484,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -481,9 +508,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,14 +531,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -514,51 +539,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -580,13 +561,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,13 +681,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,151 +729,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,21 +765,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -828,29 +794,50 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -870,24 +857,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -905,132 +886,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1057,9 +1038,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,10 +1360,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1455,7 +1433,7 @@
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1466,7 +1444,7 @@
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1517,44 +1495,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="10" t="s">
+    <row r="12" s="7" customFormat="1" spans="1:3">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" s="7" customFormat="1" spans="1:3">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="10" t="s">
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" s="7" customFormat="1" spans="1:3">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="10" t="s">
+    <row r="15" s="7" customFormat="1" spans="1:3">
+      <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -1587,7 +1565,7 @@
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1609,7 +1587,7 @@
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1621,75 +1599,75 @@
         <v>41</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" s="7" customFormat="1" spans="1:3">
-      <c r="A22" s="7" t="s">
+      <c r="B22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" s="7" customFormat="1" spans="1:3">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" s="7" customFormat="1" spans="1:3">
-      <c r="A24" s="7" t="s">
+      <c r="C24" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" s="7" customFormat="1" spans="1:3">
-      <c r="A25" s="7" t="s">
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="7" t="s">
+      <c r="B26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="C26" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1737,56 +1715,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="10" t="s">
+    <row r="32" s="7" customFormat="1" spans="1:3">
+      <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="10" t="s">
+      <c r="C32" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" s="7" customFormat="1" spans="1:3">
+      <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" display="samuelslade@bpp.com "/>
+    <hyperlink ref="B18" r:id="rId1" display="samuelslade@bpp.com "/>
     <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
-    <hyperlink ref="B24" r:id="rId1" display="neo4j"/>
-    <hyperlink ref="B26" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
+    <hyperlink ref="B20" r:id="rId1" display="neo4j"/>
+    <hyperlink ref="B22" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
+    <hyperlink ref="B32" r:id="rId4" display="nadineanja@yahoo.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1799,7 +1756,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1823,10 +1780,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1834,10 +1791,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1845,10 +1802,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1856,10 +1813,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1867,10 +1824,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1878,10 +1835,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1923,10 +1880,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1934,10 +1891,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1945,10 +1902,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1956,10 +1913,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1967,10 +1924,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1978,10 +1935,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1989,10 +1946,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2000,10 +1957,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2011,10 +1968,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2022,10 +1979,10 @@
     </row>
     <row r="11" s="4" customFormat="1" spans="1:3">
       <c r="A11" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -2033,10 +1990,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -2044,10 +2001,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -2055,10 +2012,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -2066,10 +2023,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -2077,10 +2034,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>5</v>
@@ -2088,10 +2045,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>5</v>
@@ -2099,10 +2056,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -2155,10 +2112,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2166,10 +2123,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Product Factory test fix; Separated scrollFor and scrollToElement logic in UiHandlers; ACCEPT_ALERT handler fixed: triggered only if cause is not null; SPINNER_HANDLER logic is changed; Created .checkCheckbox() overload with handlers in BasePage; Added link to new PF env. to Common_MetaData.xls; Updated version of WebDriver for Mac.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/qa-automation-framework-poc/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8A42F-2679-EE49-BBA2-4313EEE48D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28245" windowHeight="12660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28240" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="Links" sheetId="2" r:id="rId3"/>
     <sheet name="Validdata" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
   <si>
     <t>Tag</t>
   </si>
@@ -350,19 +356,19 @@
   </si>
   <si>
     <t>MSc Management CRO PTD 201819 for student application</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYURLNEW</t>
+  </si>
+  <si>
+    <t>http://pf-services-qa2-482823960.eu-west-2.elb.amazonaws.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,338 +421,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -767,249 +451,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1021,82 +466,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1354,27 +756,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1619047619048" style="10" customWidth="1"/>
-    <col min="2" max="2" width="45.5047619047619" style="10" customWidth="1"/>
-    <col min="3" max="3" width="44.1619047619048" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="8.66666666666667" style="10"/>
+    <col min="1" max="1" width="38.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1396,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -1407,7 +809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1418,7 +820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -1429,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -1440,7 +842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1451,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -1462,7 +864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -1484,7 +886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="1" spans="1:3">
+    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1506,7 +908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="1" spans="1:3">
+    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
@@ -1517,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" s="7" customFormat="1" spans="1:3">
+    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
@@ -1528,7 +930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" s="7" customFormat="1" spans="1:3">
+    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
@@ -1539,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1550,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1561,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" s="7" customFormat="1" spans="1:3">
+    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1572,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" s="7" customFormat="1" spans="1:3">
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -1583,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="1" spans="1:3">
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1594,7 +996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="1" spans="1:3">
+    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
@@ -1605,7 +1007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -1616,7 +1018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -1627,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>45</v>
       </c>
@@ -1638,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
@@ -1649,7 +1051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>49</v>
       </c>
@@ -1660,7 +1062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
@@ -1671,7 +1073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
@@ -1682,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>55</v>
       </c>
@@ -1693,7 +1095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>57</v>
       </c>
@@ -1704,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
@@ -1715,7 +1117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" s="7" customFormat="1" spans="1:3">
+    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
@@ -1726,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" s="7" customFormat="1" spans="1:3">
+    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
@@ -1739,35 +1141,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" display="samuelslade@bpp.com "/>
-    <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
-    <hyperlink ref="B20" r:id="rId1" display="neo4j"/>
-    <hyperlink ref="B22" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
-    <hyperlink ref="B32" r:id="rId4" display="nadineanja@yahoo.com"/>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B22" r:id="rId4" tooltip="mailto:craigolivant@bpp.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1789,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1800,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1811,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1822,7 +1222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1833,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1845,29 +1245,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="26.1619047619048" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -1889,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -1900,7 +1298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>78</v>
       </c>
@@ -1911,7 +1309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>80</v>
       </c>
@@ -1922,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -1933,7 +1331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>84</v>
       </c>
@@ -1944,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>86</v>
       </c>
@@ -1955,7 +1353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>88</v>
       </c>
@@ -1966,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
@@ -1977,7 +1375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:3">
+    <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>92</v>
       </c>
@@ -1988,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>94</v>
       </c>
@@ -1999,7 +1397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>96</v>
       </c>
@@ -2010,7 +1408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>98</v>
       </c>
@@ -2021,7 +1419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>100</v>
       </c>
@@ -2032,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>102</v>
       </c>
@@ -2043,7 +1441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>103</v>
       </c>
@@ -2054,7 +1452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>105</v>
       </c>
@@ -2065,41 +1463,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
-    <hyperlink ref="B3" r:id="rId1" display=" http://noahqa-bpp-13fd3e55188.cs17.force.com/rfi"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://bpp-test.apolloglobal.int/registration/login" tooltip="Follow link"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://bpp-test.apolloglobal.int/ncas"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://bpp-test.apolloglobal.int/ncas/login?service=https://bpp-fusion-test.apolloglobal.int/ncas/sso-login"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://bpp-fusion-test.apolloglobal.int/vle/login/index.php?authCAS=NOCAS"/>
-    <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
-    <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="Follow link" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B14" r:id="rId9" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="34.5047619047619" customWidth="1"/>
-    <col min="3" max="3" width="37.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2110,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>107</v>
       </c>
@@ -2121,7 +1528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -2133,7 +1540,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PF Database Cleanup scenario created; PDCleanupRunner class created; Created productFactory.xml for TestNG; Created beforeMethod for Product Factory test group
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/qa-automation-framework-poc/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8A42F-2679-EE49-BBA2-4313EEE48D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917D3DC-CC86-AC4A-B601-EC025BBE0A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28240" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
   <si>
     <t>Tag</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>http://pf-services-qa2-482823960.eu-west-2.elb.amazonaws.com/</t>
+  </si>
+  <si>
+    <t>http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYDATABASEURLNEW</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,6 +1480,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -1485,6 +1502,7 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
     <hyperlink ref="B14" r:id="rId9" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B20" r:id="rId10" xr:uid="{B2A496D7-A997-EA4A-86F0-97DC54A6149E}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Created ProductFactory.xml test suite with database cleanup before it; Updated setText() method in BasePage; Created executeJSCode() step definition; Fixed ‘Create Course Instance’ scenario; Added ff_version variable to default.properties; Changed browserStackBuild in default.properties; Fixed geckodriver path in DriverProvider; Updated geckodriver; PFCleanupRunner class created.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/qa-automation-framework-poc/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917D3DC-CC86-AC4A-B601-EC025BBE0A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C72FCD6-8D33-D840-A21E-E70F817CFAD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28240" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28240" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="120">
   <si>
     <t>Tag</t>
   </si>
@@ -368,6 +368,21 @@
   </si>
   <si>
     <t>PRODUCTFACTORYDATABASEURLNEW</t>
+  </si>
+  <si>
+    <t>SPACE</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYDATABASEUSERNEW</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYDATABASEPASSWORDNEW</t>
+  </si>
+  <si>
+    <t>Neo4j</t>
+  </si>
+  <si>
+    <t>3M#$,qns5uw*W#jr</t>
   </si>
 </sst>
 </file>
@@ -387,13 +402,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -401,14 +416,14 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -416,7 +431,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -424,7 +439,7 @@
       <sz val="11"/>
       <color rgb="FF007DD6"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -768,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1142,6 +1157,28 @@
         <v>64</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1160,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1250,6 +1287,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1260,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated test for VPE Pages; amended metadata
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/Common_MetaData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevytskyi/IdeaProjects/qa-automation-framework-poc/src/main/resources/data/bpp/keywords.metadata/metadata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9DB43B-E426-204B-BC48-5CF0832AF043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28240" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="18792" windowHeight="9487" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>Tag</t>
   </si>
@@ -220,6 +214,18 @@
     <t>Wake Up 19!</t>
   </si>
   <si>
+    <t>PRODUCTFACTORYDATABASEUSERNEW</t>
+  </si>
+  <si>
+    <t>Neo4j</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYDATABASEPASSWORDNEW</t>
+  </si>
+  <si>
+    <t>3M#$,qns5uw*W#jr</t>
+  </si>
+  <si>
     <t>ENTER</t>
   </si>
   <si>
@@ -247,6 +253,9 @@
     <t>END</t>
   </si>
   <si>
+    <t>SPACE</t>
+  </si>
+  <si>
     <t>SALESFORCEURL</t>
   </si>
   <si>
@@ -346,6 +355,18 @@
     <t>https://totara.staging.bppdigital.buildempire.app/login/index.php</t>
   </si>
   <si>
+    <t>PRODUCTFACTORYURLNEW</t>
+  </si>
+  <si>
+    <t>https://qa2-products.bpp.com/</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYDATABASEURLNEW</t>
+  </si>
+  <si>
+    <t>http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/</t>
+  </si>
+  <si>
     <t>CUSTOMERGROUP</t>
   </si>
   <si>
@@ -358,38 +379,20 @@
     <t>MSc Management CRO PTD 201819 for student application</t>
   </si>
   <si>
-    <t>PRODUCTFACTORYURLNEW</t>
-  </si>
-  <si>
-    <t>http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/</t>
-  </si>
-  <si>
-    <t>PRODUCTFACTORYDATABASEURLNEW</t>
-  </si>
-  <si>
-    <t>SPACE</t>
-  </si>
-  <si>
-    <t>PRODUCTFACTORYDATABASEUSERNEW</t>
-  </si>
-  <si>
-    <t>PRODUCTFACTORYDATABASEPASSWORDNEW</t>
-  </si>
-  <si>
-    <t>Neo4j</t>
-  </si>
-  <si>
-    <t>3M#$,qns5uw*W#jr</t>
-  </si>
-  <si>
-    <t>https://qa2-products.bpp.com/</t>
+    <t>SFOFFERING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,13 +405,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -416,14 +419,14 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,7 +434,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -439,19 +442,341 @@
       <sz val="11"/>
       <color rgb="FF007DD6"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -472,12 +797,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,40 +1050,86 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -777,27 +1387,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6605504587156" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="10"/>
+    <col min="1" max="1" width="38.1651376146789" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5045871559633" style="11" customWidth="1"/>
+    <col min="3" max="3" width="44.1651376146789" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="8.6605504587156" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,409 +1418,411 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="C8" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="C11" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" s="8" customFormat="1" spans="1:3">
+      <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" s="8" customFormat="1" spans="1:3">
+      <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" s="8" customFormat="1" spans="1:3">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" s="8" customFormat="1" spans="1:3">
+      <c r="A15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" s="8" customFormat="1" spans="1:3">
+      <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" s="8" customFormat="1" spans="1:3">
+      <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" s="8" customFormat="1" spans="1:3">
+      <c r="A18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" s="8" customFormat="1" spans="1:3">
+      <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="C19" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" s="8" customFormat="1" spans="1:3">
+      <c r="A20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="C20" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" s="8" customFormat="1" spans="1:3">
+      <c r="A21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="C21" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="C22" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="C23" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="C24" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="C25" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="C26" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="C27" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="C28" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="C29" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="C30" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="C31" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" s="8" customFormat="1" spans="1:3">
+      <c r="A32" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="C32" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" s="8" customFormat="1" spans="1:3">
+      <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="C33" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B22" r:id="rId4" tooltip="mailto:craigolivant@bpp.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B18" r:id="rId1" display="samuelslade@bpp.com "/>
+    <hyperlink ref="B4" r:id="rId2" display="crmteamfusionadmin@gmail.com.noahqa"/>
+    <hyperlink ref="B20" r:id="rId1" display="neo4j"/>
+    <hyperlink ref="B22" r:id="rId3" display="craigolivant@bpp.com" tooltip="mailto:craigolivant@bpp.com"/>
+    <hyperlink ref="B32" r:id="rId4" display="nadineanja@yahoo.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
+    <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6605504587156" customWidth="1"/>
+    <col min="2" max="2" width="26.6605504587156" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,105 +1833,107 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.6605504587156" customWidth="1"/>
+    <col min="3" max="3" width="26.1651376146789" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,249 +1944,251 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" s="5" customFormat="1" spans="1:3">
+      <c r="A11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
+      <c r="A16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" tooltip="Follow link" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B14" r:id="rId9" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="B20" r:id="rId10" xr:uid="{B2A496D7-A997-EA4A-86F0-97DC54A6149E}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://cs21.salesforce.com/home/home.jsp"/>
+    <hyperlink ref="B3" r:id="rId1" display=" http://noahqa-bpp-13fd3e55188.cs17.force.com/rfi"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://bpp-test.apolloglobal.int/registration/login" tooltip="Follow link"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://bpp-test.apolloglobal.int/ncas"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://bpp-test.apolloglobal.int/ncas/login?service=https://bpp-fusion-test.apolloglobal.int/ncas/sso-login"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage" tooltip="https://bpp-cas-test.apolloglobal.int/cas/login?service=http%3A%2F%2Fbpp-ssb-test.apolloglobal.int%3A%2Fssomanager%2Fc%2FSSB%3Fname%3Dhomepage"/>
+    <hyperlink ref="B8" r:id="rId6" display="http://bpp-fusion-test.apolloglobal.int/vle/login/index.php?authCAS=NOCAS"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://bpp-test.apolloglobal.int/openbravo/"/>
+    <hyperlink ref="B14" r:id="rId8" display="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474" tooltip="http://ec2-35-178-174-237.eu-west-2.compute.amazonaws.com:7474"/>
+    <hyperlink ref="B20" r:id="rId9" display="http://ec2-3-10-141-78.eu-west-2.compute.amazonaws.com:7474/"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6605504587156" customWidth="1"/>
+    <col min="2" max="2" width="34.5045871559633" customWidth="1"/>
+    <col min="3" max="3" width="37.6605504587156" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1583,29 +2199,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2381626</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>